<commit_message>
Updating documentation to use TOF sensor
</commit_message>
<xml_diff>
--- a/documentation/Hardware (Ceng 317)/Ceng317 Budget BWoo 2019.xlsx
+++ b/documentation/Hardware (Ceng 317)/Ceng317 Budget BWoo 2019.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\Humber\Fall 2019\Ceng 317 (Hardware)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\Github BW25\Humber_Capstone\documentation\Hardware (Ceng 317)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{D74E4D66-7A31-4352-B097-C0AA1E773AF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BB191A51-D23E-491A-9717-55CC199475BE}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{D74E4D66-7A31-4352-B097-C0AA1E773AF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{59E1C5D0-3069-4B8A-8DAA-569B04ADEBC7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50C8E5D4-B488-4860-83B5-C049BAC606B7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Cost</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Wires</t>
   </si>
   <si>
-    <t>Includes HC-SR04 ultrasonic sensor, resistors, wires, LED</t>
-  </si>
-  <si>
     <t>Brendan Woo</t>
   </si>
   <si>
@@ -109,6 +106,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Includes resistors, wires, LED</t>
+  </si>
+  <si>
+    <t>VL53L0X TOF sensor</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3317</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664D9283-9F0D-41B9-BEAB-E15C8B398BAE}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,12 +526,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -566,7 +572,7 @@
         <v>60.59</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
@@ -575,43 +581,38 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6">
-        <v>11.3</v>
+        <v>26</v>
+      </c>
+      <c r="B6" s="4">
+        <v>14.95</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" s="3">
         <f>B6*C6</f>
-        <v>11.3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
+        <v>14.95</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="G6" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="6">
-        <v>5.65</v>
+        <v>11.3</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="3">
         <f>B7*C7</f>
-        <v>5.65</v>
+        <v>11.3</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -625,128 +626,153 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4">
-        <v>2.5</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
+        <v>5.65</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" ref="D8:D12" si="0">B8*C8</f>
-        <v>2.5</v>
+        <f>B8*C8</f>
+        <v>5.65</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ref="D9:D13" si="0">B9*C9</f>
+        <v>2.5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>1.5</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <v>1.5</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B12" s="4">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="7">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="7">
         <v>85.37</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>85.37</v>
       </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="4">
-        <f>SUM(D5:D12)</f>
-        <v>169.91000000000003</v>
+      <c r="G13" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4">
+        <f>SUM(D5:D13)</f>
+        <v>184.86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{3BF84F8A-2405-40BB-AB49-D1F90339979E}"/>
-    <hyperlink ref="G12" r:id="rId2" xr:uid="{473AD881-6A12-452C-BF05-52EE8E14D602}"/>
+    <hyperlink ref="G13" r:id="rId2" xr:uid="{473AD881-6A12-452C-BF05-52EE8E14D602}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{7F661006-2A29-4D9C-8816-A17BF64EBEF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating documentation and adding presentation
</commit_message>
<xml_diff>
--- a/documentation/Hardware (Ceng 317)/Ceng317 Budget BWoo 2019.xlsx
+++ b/documentation/Hardware (Ceng 317)/Ceng317 Budget BWoo 2019.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\Github BW25\Humber_Capstone\documentation\Hardware (Ceng 317)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{D74E4D66-7A31-4352-B097-C0AA1E773AF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{59E1C5D0-3069-4B8A-8DAA-569B04ADEBC7}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{D74E4D66-7A31-4352-B097-C0AA1E773AF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA25EFEA-A8CF-4397-A309-A887D5155ABA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50C8E5D4-B488-4860-83B5-C049BAC606B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
   <si>
     <t>Cost</t>
   </si>
@@ -102,9 +103,6 @@
     <t>Current price is lower</t>
   </si>
   <si>
-    <t>Ultrasonic sensor for Resistor Value Recognizer</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -115,6 +113,30 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/3317</t>
+  </si>
+  <si>
+    <t>Supplied by prototype lab</t>
+  </si>
+  <si>
+    <t>No cost</t>
+  </si>
+  <si>
+    <t>Previously purchased</t>
+  </si>
+  <si>
+    <t>Header pin and connectors</t>
+  </si>
+  <si>
+    <t>Sayal</t>
+  </si>
+  <si>
+    <t>Total project-specific</t>
+  </si>
+  <si>
+    <t>Expected budget</t>
+  </si>
+  <si>
+    <t>TOF sensor for Resistor Value Recognizer</t>
   </si>
 </sst>
 </file>
@@ -125,7 +147,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +178,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,7 +207,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -191,6 +219,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -511,9 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664D9283-9F0D-41B9-BEAB-E15C8B398BAE}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -526,7 +557,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -572,7 +603,7 @@
         <v>60.59</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
@@ -583,7 +614,7 @@
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4">
         <v>14.95</v>
@@ -597,7 +628,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="G6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -756,7 +787,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <f>SUM(D5:D13)</f>
@@ -775,4 +806,276 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F9B5ED-8420-4D25-B7F1-13F316BC674F}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4">
+        <v>14.95</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <f>B5*C5</f>
+        <v>14.95</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
+        <v>11.3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <f>B6*C6</f>
+        <v>11.3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ref="D7:D12" si="0">B7*C7</f>
+        <v>2.5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7">
+        <f>11.13/2</f>
+        <v>5.5650000000000004</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>5.5650000000000004</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="G11" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7">
+        <v>85.37</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>85.37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="D13" s="3"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="4">
+        <f>SUM(D5:D12)</f>
+        <v>124.185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4">
+        <f>SUM(D5,D11,D12)</f>
+        <v>105.88500000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="4">
+        <f>B11</f>
+        <v>5.5650000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{622AAA70-6387-4DD4-B0CE-B81AA7AB6254}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{319DB550-8C2E-4AA7-910A-C9E6FCBACBAC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Ceng317 Budget BWoo 2019.xlsx
Updating budget for build instructions
</commit_message>
<xml_diff>
--- a/documentation/Hardware (Ceng 317)/Ceng317 Budget BWoo 2019.xlsx
+++ b/documentation/Hardware (Ceng 317)/Ceng317 Budget BWoo 2019.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\Github BW25\Humber_Capstone\documentation\Hardware (Ceng 317)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{D74E4D66-7A31-4352-B097-C0AA1E773AF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6E8D5BDC-7E09-4B6A-83B1-0DEE4AF474C5}"/>
+  <xr:revisionPtr revIDLastSave="233" documentId="8_{D74E4D66-7A31-4352-B097-C0AA1E773AF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{605D7520-4600-4B31-B560-0A343EB15B54}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{50C8E5D4-B488-4860-83B5-C049BAC606B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{50C8E5D4-B488-4860-83B5-C049BAC606B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Initial projected budget" sheetId="1" r:id="rId1"/>
-    <sheet name="Final Budget" sheetId="2" r:id="rId2"/>
+    <sheet name="Budget" sheetId="3" r:id="rId1"/>
+    <sheet name="My expected budget" sheetId="1" r:id="rId2"/>
+    <sheet name="My final Budget" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>Cost</t>
   </si>
@@ -91,9 +92,6 @@
     <t>Wires</t>
   </si>
   <si>
-    <t>Brendan Woo</t>
-  </si>
-  <si>
     <t>Raspberry Pi kit</t>
   </si>
   <si>
@@ -137,17 +135,87 @@
   </si>
   <si>
     <t>TOF sensor for Resistor Value Recognizer</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>3mm cast acrylic sheet</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2Ry0JLj</t>
+  </si>
+  <si>
+    <t>m2.5 screws</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>https://bit.ly/2t4eDuB</t>
+  </si>
+  <si>
+    <t>m2.5 nuts</t>
+  </si>
+  <si>
+    <t>http://bit.ly/35lUwpC</t>
+  </si>
+  <si>
+    <t>m2 screws</t>
+  </si>
+  <si>
+    <t>http://bit.ly/2PvBeYw</t>
+  </si>
+  <si>
+    <t>m2 nuts</t>
+  </si>
+  <si>
+    <t>http://bit.ly/355GWqq</t>
+  </si>
+  <si>
+    <t>4 pin header and 6 pin header</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2PyRhVc</t>
+  </si>
+  <si>
+    <t>VL53L0X sensor</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>4 F-F wire connectors</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2RHou3L</t>
+  </si>
+  <si>
+    <t>Canakit</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2RHTccP</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,21 +252,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -207,7 +314,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -225,6 +332,28 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -541,11 +670,223 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664D9283-9F0D-41B9-BEAB-E15C8B398BAE}">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A880E59-AE1A-49C3-ABCA-145A2042F283}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15">
+        <v>14.95</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="17">
+        <v>4</v>
+      </c>
+      <c r="C3" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="14">
+        <v>4</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0.92</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.42</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0.34</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="75.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1</v>
+      </c>
+      <c r="C7" s="18">
+        <v>19.98</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15">
+        <v>14.95</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1</v>
+      </c>
+      <c r="C9" s="18">
+        <v>6.99</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+      <c r="C10" s="15">
+        <v>85.37</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18">
+        <v>144.52000000000001</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="12"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{263D54BF-8674-4B0A-BC59-2D83D8FBC4E9}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{66DA9D21-2933-4D92-A0F2-31C6A11CF095}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{601DC03E-45E9-4642-8719-76A3C7A7825A}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{5128A666-07ED-4207-B3E1-0DB74829E91F}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{B4BA2220-8C50-465F-AB11-B352D3E6B12B}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{A357A889-D995-458D-B5B3-1D53105AD267}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{070B0DC7-0E2D-47DA-A652-83B0FB4CB9B7}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{29B47332-F0BC-47E1-AEC0-16960145DC5F}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{B51E899F-0328-41FC-AF91-67D7F6ED63CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664D9283-9F0D-41B9-BEAB-E15C8B398BAE}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,93 +900,112 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>60.59</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <f>B4*C4</f>
+        <v>60.59</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4">
-        <v>60.59</v>
+        <v>14.95</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" s="3">
         <f>B5*C5</f>
-        <v>60.59</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
+        <v>14.95</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="G5" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="4">
-        <v>14.95</v>
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
+        <v>11.3</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" s="3">
         <f>B6*C6</f>
-        <v>14.95</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="G6" s="8" t="s">
-        <v>26</v>
+        <v>11.3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="6">
-        <v>11.3</v>
+        <v>5.65</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="3">
         <f>B7*C7</f>
-        <v>11.3</v>
+        <v>5.65</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -659,41 +1019,38 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6">
-        <v>5.65</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2.5</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="3">
-        <f>B8*C8</f>
-        <v>5.65</v>
+        <f t="shared" ref="D8:D12" si="0">B8*C8</f>
+        <v>2.5</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" ref="D9:D13" si="0">B9*C9</f>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -704,17 +1061,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4">
         <v>1.5</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -725,97 +1082,76 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="B12" s="7">
+        <v>85.37</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>85.37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="G12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="7">
-        <v>85.37</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>85.37</v>
-      </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>21</v>
+      <c r="B14" s="4">
+        <f>SUM(D4:D12)</f>
+        <v>184.86</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="4">
-        <f>SUM(D5:D13)</f>
-        <v>184.86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{3BF84F8A-2405-40BB-AB49-D1F90339979E}"/>
-    <hyperlink ref="G13" r:id="rId2" xr:uid="{473AD881-6A12-452C-BF05-52EE8E14D602}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{7F661006-2A29-4D9C-8816-A17BF64EBEF6}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{3BF84F8A-2405-40BB-AB49-D1F90339979E}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{473AD881-6A12-452C-BF05-52EE8E14D602}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{7F661006-2A29-4D9C-8816-A17BF64EBEF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F9B5ED-8420-4D25-B7F1-13F316BC674F}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,207 +1166,202 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4">
+        <v>14.95</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <f>B4*C4</f>
+        <v>14.95</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="4">
-        <v>14.95</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="6">
+        <v>11.3</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" s="3">
         <f>B5*C5</f>
-        <v>14.95</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>11.3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
       <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6">
-        <v>11.3</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1.5</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <f>B6*C6</f>
-        <v>11.3</v>
+        <f t="shared" ref="D6:D9" si="0">B6*C6</f>
+        <v>1.5</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" ref="D7:D10" si="0">B7*C7</f>
-        <v>1.5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="B8" s="7">
+        <f>11.13/2</f>
+        <v>5.5650000000000004</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.5650000000000004</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="G8" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B9" s="7">
-        <f>11.13/2</f>
-        <v>5.5650000000000004</v>
-      </c>
-      <c r="C9" s="10">
+        <v>85.37</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>5.5650000000000004</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="G9" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+        <v>85.37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7">
-        <v>85.37</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>85.37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
+      <c r="D10" s="3"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="D11" s="3"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4">
+        <f>SUM(D4:D9)</f>
+        <v>118.685</v>
+      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4">
-        <f>SUM(D5:D10)</f>
-        <v>118.685</v>
-      </c>
-      <c r="C12" s="4"/>
+        <f>SUM(D4,D8,D9)</f>
+        <v>105.88500000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4">
-        <f>SUM(D5,D9,D10)</f>
-        <v>105.88500000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="4">
-        <f>B9</f>
+        <f>B8</f>
         <v>5.5650000000000004</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{622AAA70-6387-4DD4-B0CE-B81AA7AB6254}"/>
-    <hyperlink ref="G10" r:id="rId2" xr:uid="{319DB550-8C2E-4AA7-910A-C9E6FCBACBAC}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{622AAA70-6387-4DD4-B0CE-B81AA7AB6254}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{319DB550-8C2E-4AA7-910A-C9E6FCBACBAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>

</xml_diff>